<commit_message>
Mise à jour des questions
</commit_message>
<xml_diff>
--- a/Documentation/Questions.xlsx
+++ b/Documentation/Questions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\william.hausmann\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projet\LesDouzeCoupsMidi\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="275">
   <si>
     <t xml:space="preserve">De quel pays Tirana est-elle la capitale ? </t>
   </si>
@@ -600,6 +600,255 @@
   </si>
   <si>
     <t>Hongrie</t>
+  </si>
+  <si>
+    <t>Combien d'albums un chanteur doit-il vendre pour recevoir un disque d'or ?</t>
+  </si>
+  <si>
+    <t>100'000</t>
+  </si>
+  <si>
+    <t>70'000</t>
+  </si>
+  <si>
+    <t>80'000</t>
+  </si>
+  <si>
+    <t>75'000</t>
+  </si>
+  <si>
+    <t>De quel moyen de locomotion le grand bi est-il l'ancêtre ?</t>
+  </si>
+  <si>
+    <t>Le dirigeable</t>
+  </si>
+  <si>
+    <t>Le monocycle</t>
+  </si>
+  <si>
+    <t>Le trycycle</t>
+  </si>
+  <si>
+    <t>La bicyclette</t>
+  </si>
+  <si>
+    <t>Quel film d'animation a pour héros Woody le cow-boy et Buzz l'éclair ?</t>
+  </si>
+  <si>
+    <t>Cars</t>
+  </si>
+  <si>
+    <t>Robots</t>
+  </si>
+  <si>
+    <t>Small Soldiers</t>
+  </si>
+  <si>
+    <t>Toy Story</t>
+  </si>
+  <si>
+    <t>Quelle est la particularité du tonneau des Danaïdes ?</t>
+  </si>
+  <si>
+    <t>Il ne se dilate jamais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il est sans fond </t>
+  </si>
+  <si>
+    <t>Il est tout le temps ouvert</t>
+  </si>
+  <si>
+    <t>Il est en cristal</t>
+  </si>
+  <si>
+    <t>Il est sans fond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quel cavalier est le maître de Rossinante ? </t>
+  </si>
+  <si>
+    <t>Don Quichotte</t>
+  </si>
+  <si>
+    <t>Jorge Luis Borges</t>
+  </si>
+  <si>
+    <t>Günter Grass</t>
+  </si>
+  <si>
+    <t>Sirano de Bergerac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quelle est la capitale du Cameroun ? </t>
+  </si>
+  <si>
+    <t>Douala</t>
+  </si>
+  <si>
+    <t>Bertoua</t>
+  </si>
+  <si>
+    <t>Yaoundé</t>
+  </si>
+  <si>
+    <t>Luanda</t>
+  </si>
+  <si>
+    <t>Qui est la muse de l'Histoire dans la mythologie grecque ?</t>
+  </si>
+  <si>
+    <t>Clio</t>
+  </si>
+  <si>
+    <t>Calliope</t>
+  </si>
+  <si>
+    <t>Uranie</t>
+  </si>
+  <si>
+    <t>Euterpe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dans la mythologie grecque, qui est le dieu des voleurs ? </t>
+  </si>
+  <si>
+    <t>Horus</t>
+  </si>
+  <si>
+    <t>Hermès</t>
+  </si>
+  <si>
+    <t>Helheim</t>
+  </si>
+  <si>
+    <t>Hélios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quel est le véritable prénom de M. Pokora ? </t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Mathéo</t>
+  </si>
+  <si>
+    <t>Mathias</t>
+  </si>
+  <si>
+    <t>Matthieu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quel couple de petits personnages rouge et bleu s'anime en 1974 ? </t>
+  </si>
+  <si>
+    <t>Boule &amp; Bill</t>
+  </si>
+  <si>
+    <t>Titi &amp; Grosminet</t>
+  </si>
+  <si>
+    <t>Coyotte &amp; Bip bip</t>
+  </si>
+  <si>
+    <t>Chapi &amp; Chapo</t>
+  </si>
+  <si>
+    <t>Quel sirop consommez-vous si vous buvez un Monaco ?</t>
+  </si>
+  <si>
+    <t>Cerise</t>
+  </si>
+  <si>
+    <t>Framboise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menthe </t>
+  </si>
+  <si>
+    <t>Grenadine</t>
+  </si>
+  <si>
+    <t>Comment s'appelle le chevalier dans Zelda</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Zelda</t>
+  </si>
+  <si>
+    <t>Gooruk</t>
+  </si>
+  <si>
+    <t>Revali</t>
+  </si>
+  <si>
+    <t>Comment s'appelle la princesse dans Mario Galaxy</t>
+  </si>
+  <si>
+    <t>Daisy</t>
+  </si>
+  <si>
+    <t>Peach</t>
+  </si>
+  <si>
+    <t>Harmonie</t>
+  </si>
+  <si>
+    <t>Queen</t>
+  </si>
+  <si>
+    <t>Dans quoi se cache le célèbre personnage dans Metal gear solid</t>
+  </si>
+  <si>
+    <t>Un carton</t>
+  </si>
+  <si>
+    <t>Un buisson</t>
+  </si>
+  <si>
+    <t>Une cabine télephonique</t>
+  </si>
+  <si>
+    <t>Un sac de couchage</t>
+  </si>
+  <si>
+    <t>Combien y'a-t-il de pokémons dans la 1er géneration</t>
+  </si>
+  <si>
+    <t>Quel est la mascotte dans pokémon</t>
+  </si>
+  <si>
+    <t>Pikachu</t>
+  </si>
+  <si>
+    <t>Evoli</t>
+  </si>
+  <si>
+    <t>Rondoudou</t>
+  </si>
+  <si>
+    <t>Insolourdo</t>
+  </si>
+  <si>
+    <t>Un berger a 16 brebis, toutes meurent sauf 10. Combien lui en reste-t-il ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Au Japon, qu'est-ce qu'un yakuza ? </t>
+  </si>
+  <si>
+    <t>Un vendeur de drogue</t>
+  </si>
+  <si>
+    <t>Une vendeur de tapis</t>
+  </si>
+  <si>
+    <t>Un membre de la mafia</t>
+  </si>
+  <si>
+    <t>Un pilier économique</t>
   </si>
 </sst>
 </file>
@@ -917,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,6 +2021,366 @@
         <v>191</v>
       </c>
     </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>192</v>
+      </c>
+      <c r="B43" t="s">
+        <v>193</v>
+      </c>
+      <c r="C43" t="s">
+        <v>194</v>
+      </c>
+      <c r="D43" t="s">
+        <v>195</v>
+      </c>
+      <c r="E43" t="s">
+        <v>196</v>
+      </c>
+      <c r="F43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>197</v>
+      </c>
+      <c r="B44" t="s">
+        <v>198</v>
+      </c>
+      <c r="C44" t="s">
+        <v>199</v>
+      </c>
+      <c r="D44" t="s">
+        <v>200</v>
+      </c>
+      <c r="E44" t="s">
+        <v>201</v>
+      </c>
+      <c r="F44" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>202</v>
+      </c>
+      <c r="B45" t="s">
+        <v>205</v>
+      </c>
+      <c r="C45" t="s">
+        <v>203</v>
+      </c>
+      <c r="D45" t="s">
+        <v>204</v>
+      </c>
+      <c r="E45" t="s">
+        <v>206</v>
+      </c>
+      <c r="F45" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>207</v>
+      </c>
+      <c r="B46" t="s">
+        <v>208</v>
+      </c>
+      <c r="C46" t="s">
+        <v>209</v>
+      </c>
+      <c r="D46" t="s">
+        <v>210</v>
+      </c>
+      <c r="E46" t="s">
+        <v>211</v>
+      </c>
+      <c r="F46" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>213</v>
+      </c>
+      <c r="B47" t="s">
+        <v>214</v>
+      </c>
+      <c r="C47" t="s">
+        <v>215</v>
+      </c>
+      <c r="D47" t="s">
+        <v>216</v>
+      </c>
+      <c r="E47" t="s">
+        <v>217</v>
+      </c>
+      <c r="F47" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>218</v>
+      </c>
+      <c r="B48" t="s">
+        <v>219</v>
+      </c>
+      <c r="C48" t="s">
+        <v>220</v>
+      </c>
+      <c r="D48" t="s">
+        <v>221</v>
+      </c>
+      <c r="E48" t="s">
+        <v>222</v>
+      </c>
+      <c r="F48" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>223</v>
+      </c>
+      <c r="B49" t="s">
+        <v>224</v>
+      </c>
+      <c r="C49" t="s">
+        <v>225</v>
+      </c>
+      <c r="D49" t="s">
+        <v>226</v>
+      </c>
+      <c r="E49" t="s">
+        <v>227</v>
+      </c>
+      <c r="F49" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>228</v>
+      </c>
+      <c r="B50" t="s">
+        <v>229</v>
+      </c>
+      <c r="C50" t="s">
+        <v>230</v>
+      </c>
+      <c r="D50" t="s">
+        <v>231</v>
+      </c>
+      <c r="E50" t="s">
+        <v>232</v>
+      </c>
+      <c r="F50" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>233</v>
+      </c>
+      <c r="B51" t="s">
+        <v>234</v>
+      </c>
+      <c r="C51" t="s">
+        <v>237</v>
+      </c>
+      <c r="D51" t="s">
+        <v>235</v>
+      </c>
+      <c r="E51" t="s">
+        <v>236</v>
+      </c>
+      <c r="F51" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>238</v>
+      </c>
+      <c r="B52" t="s">
+        <v>239</v>
+      </c>
+      <c r="C52" t="s">
+        <v>240</v>
+      </c>
+      <c r="D52" t="s">
+        <v>241</v>
+      </c>
+      <c r="E52" t="s">
+        <v>242</v>
+      </c>
+      <c r="F52" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>243</v>
+      </c>
+      <c r="B53" t="s">
+        <v>244</v>
+      </c>
+      <c r="C53" t="s">
+        <v>245</v>
+      </c>
+      <c r="D53" t="s">
+        <v>246</v>
+      </c>
+      <c r="E53" t="s">
+        <v>247</v>
+      </c>
+      <c r="F53" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>248</v>
+      </c>
+      <c r="B54" t="s">
+        <v>249</v>
+      </c>
+      <c r="C54" t="s">
+        <v>250</v>
+      </c>
+      <c r="D54" t="s">
+        <v>251</v>
+      </c>
+      <c r="E54" t="s">
+        <v>252</v>
+      </c>
+      <c r="F54" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>253</v>
+      </c>
+      <c r="B55" t="s">
+        <v>255</v>
+      </c>
+      <c r="C55" t="s">
+        <v>254</v>
+      </c>
+      <c r="D55" t="s">
+        <v>256</v>
+      </c>
+      <c r="E55" t="s">
+        <v>257</v>
+      </c>
+      <c r="F55" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>258</v>
+      </c>
+      <c r="B56" t="s">
+        <v>259</v>
+      </c>
+      <c r="C56" t="s">
+        <v>260</v>
+      </c>
+      <c r="D56" t="s">
+        <v>261</v>
+      </c>
+      <c r="E56" t="s">
+        <v>262</v>
+      </c>
+      <c r="F56" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>263</v>
+      </c>
+      <c r="B57">
+        <v>160</v>
+      </c>
+      <c r="C57">
+        <v>151</v>
+      </c>
+      <c r="D57">
+        <v>161</v>
+      </c>
+      <c r="E57">
+        <v>150</v>
+      </c>
+      <c r="F57">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>264</v>
+      </c>
+      <c r="B58" t="s">
+        <v>265</v>
+      </c>
+      <c r="C58" t="s">
+        <v>266</v>
+      </c>
+      <c r="D58" t="s">
+        <v>267</v>
+      </c>
+      <c r="E58" t="s">
+        <v>268</v>
+      </c>
+      <c r="F58" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>269</v>
+      </c>
+      <c r="B59">
+        <v>10</v>
+      </c>
+      <c r="C59">
+        <v>6</v>
+      </c>
+      <c r="D59">
+        <v>16</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>270</v>
+      </c>
+      <c r="B60" t="s">
+        <v>271</v>
+      </c>
+      <c r="C60" t="s">
+        <v>272</v>
+      </c>
+      <c r="D60" t="s">
+        <v>273</v>
+      </c>
+      <c r="E60" t="s">
+        <v>274</v>
+      </c>
+      <c r="F60" t="s">
+        <v>273</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Encodage en UTF-8 du fichier des questions
</commit_message>
<xml_diff>
--- a/Documentation/Questions.xlsx
+++ b/Documentation/Questions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LesDouzeCoupsMidi\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projet\LesDouzeCoupsMidi\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4139,8 +4139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F300"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="F303" sqref="F303"/>
+    <sheetView tabSelected="1" topLeftCell="A256" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A297" sqref="A297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>